<commit_message>
Refactor how defaults work.
</commit_message>
<xml_diff>
--- a/Truth Tables.xlsx
+++ b/Truth Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jderry1\DropBox (External)\_Organize Me\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD06321-86C2-43F7-939F-CE2AEA1EAC5C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6620FC1E-6550-4FD7-8DBA-8598EEBA86D0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="930" windowWidth="26685" windowHeight="15330" xr2:uid="{A00115A1-F69C-48DE-A751-02D76A40BDE0}"/>
+    <workbookView xWindow="29445" yWindow="1380" windowWidth="26685" windowHeight="15330" activeTab="2" xr2:uid="{A00115A1-F69C-48DE-A751-02D76A40BDE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Subs" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1603" uniqueCount="82">
   <si>
     <t>T</t>
   </si>
@@ -146,9 +146,6 @@
     <t>notA &amp;&amp; notC</t>
   </si>
   <si>
-    <t>A &amp;&amp; notB</t>
-  </si>
-  <si>
     <t>B &amp;&amp; C</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>notAnotBC</t>
   </si>
   <si>
-    <t>notAnotBnotC</t>
-  </si>
-  <si>
     <t>ABnotCnotD</t>
   </si>
   <si>
@@ -270,6 +264,21 @@
   </si>
   <si>
     <t>notA &amp;&amp; D</t>
+  </si>
+  <si>
+    <t>notBnotC</t>
+  </si>
+  <si>
+    <t>(contiguous wraps)</t>
+  </si>
+  <si>
+    <t>(continuous, wraps)</t>
+  </si>
+  <si>
+    <t>notB</t>
+  </si>
+  <si>
+    <t>AnotBC</t>
   </si>
 </sst>
 </file>
@@ -332,11 +341,6 @@
       </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
@@ -346,6 +350,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="gray125">
+        <bgColor theme="9" tint="0.59999389629810485"/>
       </patternFill>
     </fill>
   </fills>
@@ -441,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -495,19 +504,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="1" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -575,19 +578,43 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -906,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E955A30E-749C-4FFC-A339-BFF504460588}">
   <dimension ref="B2:M60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -947,7 +974,7 @@
         <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="5"/>
     </row>
@@ -974,7 +1001,7 @@
     </row>
     <row r="11" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="5"/>
     </row>
@@ -1549,33 +1576,33 @@
       <c r="C35" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D35" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="E35" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G35" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="H35" s="30" t="s">
-        <v>22</v>
+      <c r="D35" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="58" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="59" t="s">
+        <v>0</v>
+      </c>
+      <c r="G35" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>23</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C36" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="E36" s="29" t="s">
+      <c r="D36" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="27" t="s">
         <v>0</v>
       </c>
       <c r="F36" s="15" t="s">
@@ -1584,11 +1611,11 @@
       <c r="G36" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H36" s="30" t="s">
-        <v>23</v>
+      <c r="H36" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="I36" s="5" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.2">
@@ -1607,11 +1634,8 @@
       <c r="G37" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="H37" s="30" t="s">
-        <v>34</v>
-      </c>
       <c r="I37" s="5" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.2">
@@ -1630,7 +1654,7 @@
       <c r="G38" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="H38" s="30"/>
+      <c r="H38" s="28"/>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C41" s="6" t="s">
@@ -1686,11 +1710,11 @@
       <c r="G48" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="H48" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.2">
@@ -1703,13 +1727,13 @@
       <c r="E49" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F49" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G49" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H49" s="30" t="s">
+      <c r="F49" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G49" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="28" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1723,13 +1747,13 @@
       <c r="E50" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="F50" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G50" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="H50" s="30" t="s">
+      <c r="F50" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G50" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="H50" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1749,7 +1773,7 @@
       <c r="G51" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="H51" s="30"/>
+      <c r="H51" s="28"/>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C54" s="6" t="s">
@@ -1789,11 +1813,11 @@
       <c r="G56" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H56" s="28" t="s">
         <v>22</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.2">
@@ -1812,18 +1836,18 @@
       <c r="G57" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H57" s="28" t="s">
         <v>23</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C58" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="D58" s="31" t="s">
         <v>1</v>
       </c>
       <c r="E58" s="15" t="s">
@@ -1835,7 +1859,7 @@
       <c r="G58" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H58" s="28" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1855,11 +1879,11 @@
       <c r="G59" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="H59" s="30"/>
-      <c r="J59" s="34"/>
+      <c r="H59" s="28"/>
+      <c r="J59" s="32"/>
     </row>
     <row r="60" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="J60" s="34"/>
+      <c r="J60" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1871,7 +1895,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0991ABC-6BEE-4802-A3F9-177D100EDA45}">
   <dimension ref="B2:O119"/>
   <sheetViews>
-    <sheetView topLeftCell="A65" workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="M100" sqref="M100"/>
     </sheetView>
   </sheetViews>
@@ -1888,7 +1912,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="33" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1900,13 +1924,13 @@
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>42</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>1</v>
@@ -1918,29 +1942,29 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D5" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="E5" s="36" t="s">
+      <c r="D5" s="34" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="34" t="s">
         <v>4</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="34" t="s">
         <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="36"/>
+      <c r="I5" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -1949,15 +1973,15 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>55</v>
+      <c r="B11" s="35" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="37"/>
+      <c r="B12" s="35"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="37"/>
+      <c r="B13" s="35"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
@@ -1966,25 +1990,25 @@
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C17" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="34" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="H17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="H17" s="36" t="s">
+      <c r="I17" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="K17" s="5" t="s">
         <v>12</v>
@@ -2034,13 +2058,13 @@
         <f>IF(MID($C18,6,1)="0","F","T")</f>
         <v>F</v>
       </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41" t="s">
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N18" s="39"/>
+      <c r="O18" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2076,13 +2100,13 @@
         <f t="shared" ref="I19:I50" si="5">IF(MID($C19,6,1)="0","F","T")</f>
         <v>T</v>
       </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="41"/>
-      <c r="O19" s="41" t="s">
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="39"/>
+      <c r="O19" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2118,13 +2142,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41" t="s">
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N20" s="39"/>
+      <c r="O20" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2160,13 +2184,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N21" s="41"/>
-      <c r="O21" s="41" t="s">
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2202,15 +2226,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41"/>
-      <c r="M22" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O22" s="41" t="s">
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O22" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2246,15 +2270,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O23" s="41" t="s">
+      <c r="K23" s="39"/>
+      <c r="L23" s="39"/>
+      <c r="M23" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O23" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2290,15 +2314,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O24" s="41" t="s">
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
+      <c r="M24" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O24" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2334,15 +2358,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N25" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O25" s="41" t="s">
+      <c r="K25" s="39"/>
+      <c r="L25" s="39"/>
+      <c r="M25" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O25" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2378,13 +2402,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41" t="s">
+      <c r="K26" s="39"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2420,13 +2444,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N27" s="41"/>
-      <c r="O27" s="41" t="s">
+      <c r="K27" s="39"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2462,13 +2486,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41"/>
-      <c r="M28" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N28" s="41"/>
-      <c r="O28" s="41" t="s">
+      <c r="K28" s="39"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2504,13 +2528,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N29" s="41"/>
-      <c r="O29" s="41" t="s">
+      <c r="K29" s="39"/>
+      <c r="L29" s="39"/>
+      <c r="M29" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2546,15 +2570,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N30" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O30" s="41" t="s">
+      <c r="K30" s="39"/>
+      <c r="L30" s="39"/>
+      <c r="M30" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O30" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2590,15 +2614,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
-      <c r="M31" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N31" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O31" s="41" t="s">
+      <c r="K31" s="39"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2634,15 +2658,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
-      <c r="M32" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N32" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O32" s="41" t="s">
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O32" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2678,15 +2702,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N33" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O33" s="41" t="s">
+      <c r="K33" s="39"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O33" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2722,13 +2746,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="41" t="s">
+      <c r="K34" s="39"/>
+      <c r="L34" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2764,13 +2788,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41"/>
-      <c r="O35" s="41" t="s">
+      <c r="K35" s="39"/>
+      <c r="L35" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2806,13 +2830,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41"/>
-      <c r="O36" s="41" t="s">
+      <c r="K36" s="39"/>
+      <c r="L36" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2848,13 +2872,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41"/>
-      <c r="O37" s="41" t="s">
+      <c r="K37" s="39"/>
+      <c r="L37" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39"/>
+      <c r="O37" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2890,15 +2914,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K38" s="41"/>
-      <c r="L38" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M38" s="41"/>
-      <c r="N38" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O38" s="41" t="s">
+      <c r="K38" s="39"/>
+      <c r="L38" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2934,15 +2958,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M39" s="41"/>
-      <c r="N39" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O39" s="41" t="s">
+      <c r="K39" s="39"/>
+      <c r="L39" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O39" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2978,15 +3002,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K40" s="41"/>
-      <c r="L40" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M40" s="41"/>
-      <c r="N40" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O40" s="41" t="s">
+      <c r="K40" s="39"/>
+      <c r="L40" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M40" s="39"/>
+      <c r="N40" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O40" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3022,15 +3046,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O41" s="41" t="s">
+      <c r="K41" s="39"/>
+      <c r="L41" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O41" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3066,13 +3090,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K42" s="41"/>
-      <c r="L42" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
-      <c r="O42" s="41"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
+      <c r="O42" s="39"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B43" s="5">
@@ -3106,13 +3130,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K43" s="41"/>
-      <c r="L43" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M43" s="41"/>
-      <c r="N43" s="41"/>
-      <c r="O43" s="41" t="s">
+      <c r="K43" s="39"/>
+      <c r="L43" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39"/>
+      <c r="O43" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3148,13 +3172,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K44" s="41"/>
-      <c r="L44" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41"/>
-      <c r="O44" s="41" t="s">
+      <c r="K44" s="39"/>
+      <c r="L44" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39"/>
+      <c r="O44" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3190,13 +3214,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="41" t="s">
+      <c r="K45" s="39"/>
+      <c r="L45" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39"/>
+      <c r="O45" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3232,15 +3256,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K46" s="41"/>
-      <c r="L46" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M46" s="41"/>
-      <c r="N46" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O46" s="41" t="s">
+      <c r="K46" s="39"/>
+      <c r="L46" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M46" s="39"/>
+      <c r="N46" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O46" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3276,15 +3300,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K47" s="41"/>
-      <c r="L47" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M47" s="41"/>
-      <c r="N47" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O47" s="41" t="s">
+      <c r="K47" s="39"/>
+      <c r="L47" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" s="39"/>
+      <c r="N47" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O47" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3320,15 +3344,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K48" s="41"/>
-      <c r="L48" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O48" s="41" t="s">
+      <c r="K48" s="39"/>
+      <c r="L48" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M48" s="39"/>
+      <c r="N48" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3364,15 +3388,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="K49" s="41"/>
-      <c r="L49" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M49" s="41"/>
-      <c r="N49" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="O49" s="41" t="s">
+      <c r="K49" s="39"/>
+      <c r="L49" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" s="39"/>
+      <c r="N49" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="O49" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3408,23 +3432,23 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="K50" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
-      <c r="O50" s="41" t="s">
+      <c r="K50" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
+      <c r="O50" s="39" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B51" s="30" t="s">
-        <v>63</v>
+      <c r="B51" s="28" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B57" s="37"/>
+      <c r="B57" s="35"/>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C58" s="6" t="s">
@@ -3433,36 +3457,36 @@
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D59" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D59" s="9" t="s">
+      <c r="E59" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="F59" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="G59" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G59" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H59" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I59" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I59" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J59" s="41">
+      <c r="J59" s="39">
         <v>101</v>
       </c>
-      <c r="K59" s="41">
+      <c r="K59" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C60" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D60" s="11"/>
       <c r="E60" s="12"/>
@@ -3475,7 +3499,7 @@
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C61" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="15"/>
@@ -3485,7 +3509,7 @@
       <c r="I61" s="15"/>
       <c r="J61" s="15"/>
       <c r="K61" s="16"/>
-      <c r="L61" s="30" t="s">
+      <c r="L61" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M61" s="5" t="s">
@@ -3494,7 +3518,7 @@
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C62" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="15"/>
@@ -3507,7 +3531,7 @@
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C63" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D63" s="14"/>
       <c r="E63" s="15"/>
@@ -3520,117 +3544,117 @@
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C64" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J64" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K64" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J64" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K64" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="65" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C65" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D65" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J65" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K65" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J65" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C66" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="D66" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J66" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K66" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D66" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J66" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K66" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C67" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D67" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="E67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="F67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="G67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="H67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="I67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="J67" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="K67" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D67" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="E67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="G67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J67" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="K67" s="42" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3641,36 +3665,36 @@
     </row>
     <row r="72" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C72" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D72" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D72" s="9" t="s">
+      <c r="E72" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E72" s="9" t="s">
+      <c r="F72" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F72" s="9" t="s">
+      <c r="G72" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G72" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H72" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I72" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I72" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J72" s="41">
+      <c r="J72" s="39">
         <v>101</v>
       </c>
-      <c r="K72" s="41">
+      <c r="K72" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="73" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C73" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D73" s="11"/>
       <c r="E73" s="12"/>
@@ -3683,7 +3707,7 @@
     </row>
     <row r="74" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C74" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D74" s="14"/>
       <c r="E74" s="15"/>
@@ -3693,74 +3717,74 @@
       <c r="I74" s="15"/>
       <c r="J74" s="15"/>
       <c r="K74" s="16"/>
-      <c r="L74" s="30" t="s">
+      <c r="L74" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M74" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C75" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D75" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J75" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K75" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D75" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J75" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K75" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="76" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C76" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D76" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J76" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K76" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J76" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K76" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="77" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C77" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D77" s="14"/>
       <c r="E77" s="15"/>
@@ -3773,7 +3797,7 @@
     </row>
     <row r="78" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C78" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D78" s="14"/>
       <c r="E78" s="15"/>
@@ -3786,7 +3810,7 @@
     </row>
     <row r="79" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C79" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D79" s="14"/>
       <c r="E79" s="15"/>
@@ -3799,7 +3823,7 @@
     </row>
     <row r="80" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C80" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="18"/>
@@ -3817,36 +3841,36 @@
     </row>
     <row r="85" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C85" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D85" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D85" s="9" t="s">
+      <c r="E85" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E85" s="9" t="s">
+      <c r="F85" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F85" s="9" t="s">
+      <c r="G85" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G85" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H85" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I85" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I85" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J85" s="41">
+      <c r="J85" s="39">
         <v>101</v>
       </c>
-      <c r="K85" s="41">
+      <c r="K85" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="86" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C86" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D86" s="20" t="s">
         <v>0</v>
@@ -3875,33 +3899,33 @@
     </row>
     <row r="87" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C87" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D87" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J87" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K87" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="L87" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J87" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K87" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="L87" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M87" s="5" t="s">
@@ -3910,7 +3934,7 @@
     </row>
     <row r="88" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C88" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D88" s="14"/>
       <c r="E88" s="15"/>
@@ -3923,7 +3947,7 @@
     </row>
     <row r="89" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C89" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D89" s="14"/>
       <c r="E89" s="15"/>
@@ -3936,7 +3960,7 @@
     </row>
     <row r="90" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C90" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D90" s="14"/>
       <c r="E90" s="15"/>
@@ -3949,7 +3973,7 @@
     </row>
     <row r="91" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C91" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D91" s="14"/>
       <c r="E91" s="15"/>
@@ -3962,7 +3986,7 @@
     </row>
     <row r="92" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C92" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D92" s="14"/>
       <c r="E92" s="15"/>
@@ -3975,7 +3999,7 @@
     </row>
     <row r="93" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C93" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D93" s="17"/>
       <c r="E93" s="18"/>
@@ -3993,36 +4017,36 @@
     </row>
     <row r="98" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C98" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D98" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D98" s="9" t="s">
+      <c r="E98" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E98" s="9" t="s">
+      <c r="F98" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F98" s="9" t="s">
+      <c r="G98" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G98" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H98" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I98" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I98" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J98" s="41">
+      <c r="J98" s="39">
         <v>101</v>
       </c>
-      <c r="K98" s="41">
+      <c r="K98" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="99" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C99" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D99" s="11"/>
       <c r="E99" s="12"/>
@@ -4040,79 +4064,79 @@
       <c r="K99" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="L99" s="30" t="s">
+      <c r="L99" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M99" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="100" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C100" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D100" s="14"/>
       <c r="E100" s="15"/>
       <c r="F100" s="15"/>
       <c r="G100" s="15"/>
-      <c r="H100" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I100" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J100" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K100" s="32" t="s">
+      <c r="H100" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I100" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J100" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K100" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="101" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C101" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D101" s="14"/>
       <c r="E101" s="15"/>
       <c r="F101" s="15"/>
       <c r="G101" s="15"/>
-      <c r="H101" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I101" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J101" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K101" s="32" t="s">
+      <c r="H101" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I101" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J101" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K101" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="102" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C102" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="15"/>
       <c r="F102" s="15"/>
       <c r="G102" s="15"/>
-      <c r="H102" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I102" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J102" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K102" s="32" t="s">
+      <c r="H102" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I102" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J102" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K102" s="30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="103" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C103" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D103" s="14"/>
       <c r="E103" s="15"/>
@@ -4125,7 +4149,7 @@
     </row>
     <row r="104" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C104" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D104" s="14"/>
       <c r="E104" s="15"/>
@@ -4138,7 +4162,7 @@
     </row>
     <row r="105" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C105" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D105" s="14"/>
       <c r="E105" s="15"/>
@@ -4151,7 +4175,7 @@
     </row>
     <row r="106" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C106" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D106" s="17"/>
       <c r="E106" s="18"/>
@@ -4169,36 +4193,36 @@
     </row>
     <row r="111" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C111" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D111" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D111" s="9" t="s">
+      <c r="E111" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E111" s="9" t="s">
+      <c r="F111" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F111" s="9" t="s">
+      <c r="G111" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G111" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H111" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I111" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I111" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J111" s="41">
+      <c r="J111" s="39">
         <v>101</v>
       </c>
-      <c r="K111" s="41">
+      <c r="K111" s="39">
         <v>100</v>
       </c>
     </row>
     <row r="112" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C112" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D112" s="11" t="s">
         <v>0</v>
@@ -4227,7 +4251,7 @@
     </row>
     <row r="113" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C113" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D113" s="14" t="s">
         <v>0</v>
@@ -4253,18 +4277,18 @@
       <c r="K113" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="L113" s="30" t="s">
+      <c r="L113" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M113" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="114" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C114" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D114" s="33"/>
+        <v>45</v>
+      </c>
+      <c r="D114" s="31"/>
       <c r="E114" s="15" t="s">
         <v>0</v>
       </c>
@@ -4287,12 +4311,12 @@
         <v>0</v>
       </c>
       <c r="M114" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="115" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C115" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D115" s="14" t="s">
         <v>0</v>
@@ -4321,7 +4345,7 @@
     </row>
     <row r="116" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C116" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D116" s="14" t="s">
         <v>0</v>
@@ -4350,7 +4374,7 @@
     </row>
     <row r="117" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C117" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D117" s="14" t="s">
         <v>0</v>
@@ -4379,7 +4403,7 @@
     </row>
     <row r="118" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C118" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D118" s="14" t="s">
         <v>0</v>
@@ -4408,7 +4432,7 @@
     </row>
     <row r="119" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C119" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D119" s="17" t="s">
         <v>0</v>
@@ -4445,8 +4469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C22A146-54CD-4232-A44B-B3773BDE98DF}">
   <dimension ref="B2:N99"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="M81" sqref="M81"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="M71" sqref="M71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4462,8 +4486,8 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="35" t="s">
-        <v>67</v>
+      <c r="B2" s="33" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
@@ -4474,13 +4498,13 @@
         <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -4489,26 +4513,26 @@
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="34" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="34" t="s">
         <v>5</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="36"/>
+      <c r="H5" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="J5" s="34"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -4517,15 +4541,15 @@
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
-        <v>69</v>
+      <c r="B11" s="35" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="37"/>
+      <c r="B12" s="35"/>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="37"/>
+      <c r="B13" s="35"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="6" t="s">
@@ -4534,22 +4558,22 @@
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="34" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D17" s="36" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="5" t="s">
+      <c r="G17" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="H17" s="5" t="s">
         <v>59</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>60</v>
       </c>
       <c r="J17" s="5" t="s">
         <v>12</v>
@@ -4595,13 +4619,13 @@
         <f>IF(MID($C18,5,1)="0","F","T")</f>
         <v>F</v>
       </c>
-      <c r="J18" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41" t="s">
+      <c r="J18" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K18" s="39"/>
+      <c r="L18" s="39"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4633,13 +4657,13 @@
         <f t="shared" ref="H19:H49" si="5">IF(MID($C19,5,1)="0","F","T")</f>
         <v>T</v>
       </c>
-      <c r="J19" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K19" s="41"/>
-      <c r="L19" s="41"/>
-      <c r="M19" s="41"/>
-      <c r="N19" s="41" t="s">
+      <c r="J19" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K19" s="39"/>
+      <c r="L19" s="39"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4671,13 +4695,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J20" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41" t="s">
+      <c r="J20" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K20" s="39"/>
+      <c r="L20" s="39"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4709,13 +4733,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J21" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41" t="s">
+      <c r="J21" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4747,15 +4771,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M22" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N22" s="41" t="s">
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M22" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N22" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4787,15 +4811,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J23" s="41"/>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M23" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N23" s="41" t="s">
+      <c r="J23" s="39"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M23" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N23" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4827,15 +4851,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M24" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N24" s="41" t="s">
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N24" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4867,15 +4891,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M25" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N25" s="41" t="s">
+      <c r="J25" s="39"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N25" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4907,13 +4931,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41" t="s">
+      <c r="J26" s="39"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4945,13 +4969,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41" t="s">
+      <c r="J27" s="39"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -4983,13 +5007,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J28" s="41"/>
-      <c r="K28" s="41"/>
-      <c r="L28" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M28" s="41"/>
-      <c r="N28" s="41" t="s">
+      <c r="J28" s="39"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5021,13 +5045,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41" t="s">
+      <c r="J29" s="39"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M29" s="39"/>
+      <c r="N29" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5059,15 +5083,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M30" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N30" s="41" t="s">
+      <c r="J30" s="39"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M30" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N30" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5099,15 +5123,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M31" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N31" s="41" t="s">
+      <c r="J31" s="39"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N31" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5139,15 +5163,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M32" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N32" s="41" t="s">
+      <c r="J32" s="39"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M32" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N32" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5179,15 +5203,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="M33" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N33" s="41" t="s">
+      <c r="J33" s="39"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="M33" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N33" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5219,13 +5243,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J34" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41" t="s">
+      <c r="J34" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5257,13 +5281,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J35" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K35" s="41"/>
-      <c r="L35" s="41"/>
-      <c r="M35" s="41"/>
-      <c r="N35" s="41" t="s">
+      <c r="J35" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5295,13 +5319,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J36" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K36" s="41"/>
-      <c r="L36" s="41"/>
-      <c r="M36" s="41"/>
-      <c r="N36" s="41" t="s">
+      <c r="J36" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K36" s="39"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5333,13 +5357,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J37" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="K37" s="41"/>
-      <c r="L37" s="41"/>
-      <c r="M37" s="41"/>
-      <c r="N37" s="41" t="s">
+      <c r="J37" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="K37" s="39"/>
+      <c r="L37" s="39"/>
+      <c r="M37" s="39"/>
+      <c r="N37" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5371,15 +5395,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J38" s="41"/>
-      <c r="K38" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L38" s="41"/>
-      <c r="M38" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N38" s="41" t="s">
+      <c r="J38" s="39"/>
+      <c r="K38" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N38" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5411,15 +5435,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N39" s="41" t="s">
+      <c r="J39" s="39"/>
+      <c r="K39" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N39" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5451,15 +5475,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J40" s="41"/>
-      <c r="K40" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L40" s="41"/>
-      <c r="M40" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N40" s="41" t="s">
+      <c r="J40" s="39"/>
+      <c r="K40" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L40" s="39"/>
+      <c r="M40" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5491,15 +5515,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L41" s="41"/>
-      <c r="M41" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N41" s="41" t="s">
+      <c r="J41" s="39"/>
+      <c r="K41" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="39"/>
+      <c r="M41" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5531,13 +5555,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J42" s="41"/>
-      <c r="K42" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L42" s="41"/>
-      <c r="M42" s="41"/>
-      <c r="N42" s="41"/>
+      <c r="J42" s="39"/>
+      <c r="K42" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L42" s="39"/>
+      <c r="M42" s="39"/>
+      <c r="N42" s="39"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="5">
@@ -5567,13 +5591,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L43" s="41"/>
-      <c r="M43" s="41"/>
-      <c r="N43" s="41" t="s">
+      <c r="J43" s="39"/>
+      <c r="K43" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L43" s="39"/>
+      <c r="M43" s="39"/>
+      <c r="N43" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5605,13 +5629,13 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J44" s="41"/>
-      <c r="K44" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L44" s="41"/>
-      <c r="M44" s="41"/>
-      <c r="N44" s="41" t="s">
+      <c r="J44" s="39"/>
+      <c r="K44" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L44" s="39"/>
+      <c r="M44" s="39"/>
+      <c r="N44" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5643,13 +5667,13 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L45" s="41"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41" t="s">
+      <c r="J45" s="39"/>
+      <c r="K45" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L45" s="39"/>
+      <c r="M45" s="39"/>
+      <c r="N45" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5681,15 +5705,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J46" s="41"/>
-      <c r="K46" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L46" s="41"/>
-      <c r="M46" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N46" s="41" t="s">
+      <c r="J46" s="39"/>
+      <c r="K46" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L46" s="39"/>
+      <c r="M46" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N46" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5721,15 +5745,15 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L47" s="41"/>
-      <c r="M47" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N47" s="41" t="s">
+      <c r="J47" s="39"/>
+      <c r="K47" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L47" s="39"/>
+      <c r="M47" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5761,15 +5785,15 @@
         <f t="shared" si="5"/>
         <v>F</v>
       </c>
-      <c r="J48" s="41"/>
-      <c r="K48" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N48" s="41" t="s">
+      <c r="J48" s="39"/>
+      <c r="K48" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L48" s="39"/>
+      <c r="M48" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="39" t="s">
         <v>0</v>
       </c>
     </row>
@@ -5801,31 +5825,31 @@
         <f t="shared" si="5"/>
         <v>T</v>
       </c>
-      <c r="J49" s="41"/>
-      <c r="K49" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="L49" s="41"/>
-      <c r="M49" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="N49" s="41" t="s">
+      <c r="J49" s="39"/>
+      <c r="K49" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="39"/>
+      <c r="M49" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" s="39" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C50" s="7"/>
-      <c r="J50" s="41"/>
-      <c r="K50" s="41"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
+      <c r="J50" s="39"/>
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="39"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="30"/>
+      <c r="B51" s="28"/>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B57" s="37"/>
+      <c r="B57" s="35"/>
     </row>
     <row r="58" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C58" s="6" t="s">
@@ -5834,30 +5858,30 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C59" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D59" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="F59" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F59" s="9" t="s">
+      <c r="G59" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G59" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H59" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I59" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I59" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J59" s="41">
+      <c r="J59" s="39">
         <v>101</v>
       </c>
-      <c r="K59" s="41">
+      <c r="K59" s="39">
         <v>100</v>
       </c>
     </row>
@@ -5865,81 +5889,78 @@
       <c r="C60" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D60" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F60" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G60" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H60" s="39"/>
-      <c r="I60" s="39"/>
-      <c r="J60" s="39"/>
-      <c r="K60" s="40"/>
+      <c r="D60" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="E60" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="F60" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="G60" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="H60" s="37"/>
+      <c r="I60" s="37"/>
+      <c r="J60" s="37"/>
+      <c r="K60" s="38"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C61" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D61" s="45"/>
-      <c r="E61" s="46"/>
-      <c r="F61" s="46"/>
-      <c r="G61" s="46"/>
-      <c r="H61" s="46"/>
-      <c r="I61" s="46"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="47"/>
-      <c r="L61" s="30" t="s">
-        <v>22</v>
+      <c r="D61" s="43"/>
+      <c r="E61" s="44"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="45"/>
+      <c r="L61" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="M61" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C62" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="46"/>
-      <c r="F62" s="46"/>
-      <c r="G62" s="46"/>
-      <c r="H62" s="46"/>
-      <c r="I62" s="46"/>
-      <c r="J62" s="46"/>
-      <c r="K62" s="47"/>
-      <c r="L62" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>39</v>
+      <c r="D62" s="43"/>
+      <c r="E62" s="44"/>
+      <c r="F62" s="44"/>
+      <c r="G62" s="44"/>
+      <c r="H62" s="44"/>
+      <c r="I62" s="44"/>
+      <c r="J62" s="44"/>
+      <c r="K62" s="45"/>
+      <c r="M62" s="56" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C63" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D63" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="E63" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="F63" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="G63" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
-      <c r="J63" s="49"/>
-      <c r="K63" s="50"/>
+      <c r="D63" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="E63" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="G63" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="48"/>
     </row>
     <row r="67" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C67" s="6" t="s">
@@ -5948,30 +5969,30 @@
     </row>
     <row r="68" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C68" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D68" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E68" s="9" t="s">
+      <c r="F68" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F68" s="9" t="s">
+      <c r="G68" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G68" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H68" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I68" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I68" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J68" s="41">
+      <c r="J68" s="39">
         <v>101</v>
       </c>
-      <c r="K68" s="41">
+      <c r="K68" s="39">
         <v>100</v>
       </c>
     </row>
@@ -5979,28 +6000,28 @@
       <c r="C69" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D69" s="38"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="39"/>
-      <c r="G69" s="39"/>
-      <c r="H69" s="39"/>
-      <c r="I69" s="39"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="40"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="37"/>
+      <c r="G69" s="37"/>
+      <c r="H69" s="37"/>
+      <c r="I69" s="37"/>
+      <c r="J69" s="37"/>
+      <c r="K69" s="38"/>
     </row>
     <row r="70" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C70" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D70" s="45"/>
-      <c r="E70" s="46"/>
-      <c r="F70" s="46"/>
-      <c r="G70" s="46"/>
-      <c r="H70" s="46"/>
-      <c r="I70" s="46"/>
-      <c r="J70" s="46"/>
-      <c r="K70" s="47"/>
-      <c r="L70" s="30" t="s">
+      <c r="D70" s="43"/>
+      <c r="E70" s="44"/>
+      <c r="F70" s="44"/>
+      <c r="G70" s="44"/>
+      <c r="H70" s="44"/>
+      <c r="I70" s="44"/>
+      <c r="J70" s="44"/>
+      <c r="K70" s="45"/>
+      <c r="L70" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M70" s="5" t="s">
@@ -6011,57 +6032,57 @@
       <c r="C71" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D71" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="E71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="F71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="G71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J71" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K71" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="L71" s="30" t="s">
+      <c r="D71" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J71" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K71" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="L71" s="28" t="s">
         <v>34</v>
       </c>
       <c r="M71" s="5" t="s">
-        <v>39</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C72" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D72" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="E72" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="F72" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="G72" s="55" t="s">
-        <v>0</v>
-      </c>
-      <c r="H72" s="49"/>
-      <c r="I72" s="49"/>
-      <c r="J72" s="49"/>
-      <c r="K72" s="50"/>
+      <c r="D72" s="46"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="47"/>
+      <c r="G72" s="47"/>
+      <c r="H72" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="I72" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="J72" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="K72" s="61" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C76" s="6" t="s">
@@ -6070,30 +6091,30 @@
     </row>
     <row r="77" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C77" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D77" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E77" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="F77" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F77" s="9" t="s">
+      <c r="G77" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G77" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H77" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I77" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I77" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J77" s="41">
+      <c r="J77" s="39">
         <v>101</v>
       </c>
-      <c r="K77" s="41">
+      <c r="K77" s="39">
         <v>100</v>
       </c>
     </row>
@@ -6101,10 +6122,10 @@
       <c r="C78" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D78" s="38"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="39"/>
-      <c r="G78" s="39"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="37"/>
+      <c r="G78" s="37"/>
       <c r="H78" s="21" t="s">
         <v>0</v>
       </c>
@@ -6122,68 +6143,68 @@
       <c r="C79" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D79" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="E79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="F79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="H79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="I79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="J79" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="K79" s="53" t="s">
-        <v>0</v>
-      </c>
-      <c r="L79" s="30" t="s">
+      <c r="D79" s="49" t="s">
+        <v>0</v>
+      </c>
+      <c r="E79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="F79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="G79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="H79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="I79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="J79" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="K79" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="L79" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M79" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C80" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D80" s="45"/>
-      <c r="E80" s="46"/>
-      <c r="F80" s="46"/>
-      <c r="G80" s="46"/>
-      <c r="H80" s="46"/>
-      <c r="I80" s="46"/>
-      <c r="J80" s="46"/>
-      <c r="K80" s="47"/>
-      <c r="L80" s="30" t="s">
+      <c r="D80" s="43"/>
+      <c r="E80" s="44"/>
+      <c r="F80" s="44"/>
+      <c r="G80" s="44"/>
+      <c r="H80" s="44"/>
+      <c r="I80" s="44"/>
+      <c r="J80" s="44"/>
+      <c r="K80" s="45"/>
+      <c r="L80" s="28" t="s">
         <v>34</v>
       </c>
       <c r="M80" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="81" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C81" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="48"/>
-      <c r="E81" s="49"/>
-      <c r="F81" s="49"/>
-      <c r="G81" s="49"/>
-      <c r="H81" s="49"/>
-      <c r="I81" s="49"/>
-      <c r="J81" s="49"/>
-      <c r="K81" s="50"/>
+      <c r="D81" s="46"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="47"/>
+      <c r="G81" s="47"/>
+      <c r="H81" s="47"/>
+      <c r="I81" s="47"/>
+      <c r="J81" s="47"/>
+      <c r="K81" s="48"/>
     </row>
     <row r="85" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C85" s="6" t="s">
@@ -6192,30 +6213,30 @@
     </row>
     <row r="86" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C86" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D86" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="F86" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="G86" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G86" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H86" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I86" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I86" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J86" s="41">
+      <c r="J86" s="39">
         <v>101</v>
       </c>
-      <c r="K86" s="41">
+      <c r="K86" s="39">
         <v>100</v>
       </c>
     </row>
@@ -6223,10 +6244,10 @@
       <c r="C87" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D87" s="38"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="39"/>
-      <c r="G87" s="39"/>
+      <c r="D87" s="36"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="37"/>
+      <c r="G87" s="37"/>
       <c r="H87" s="21" t="s">
         <v>0</v>
       </c>
@@ -6239,31 +6260,31 @@
       <c r="K87" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="L87" s="30" t="s">
+      <c r="L87" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M87" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="88" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C88" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D88" s="45"/>
-      <c r="E88" s="46"/>
-      <c r="F88" s="46"/>
-      <c r="G88" s="46"/>
-      <c r="H88" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I88" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J88" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K88" s="32" t="s">
+      <c r="D88" s="43"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
+      <c r="G88" s="44"/>
+      <c r="H88" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I88" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J88" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K88" s="30" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6271,20 +6292,20 @@
       <c r="C89" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D89" s="45"/>
-      <c r="E89" s="46"/>
-      <c r="F89" s="46"/>
-      <c r="G89" s="46"/>
-      <c r="H89" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="I89" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="J89" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="K89" s="32" t="s">
+      <c r="D89" s="43"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
+      <c r="G89" s="44"/>
+      <c r="H89" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="I89" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="J89" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="K89" s="30" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6292,20 +6313,20 @@
       <c r="C90" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D90" s="48"/>
-      <c r="E90" s="49"/>
-      <c r="F90" s="49"/>
-      <c r="G90" s="49"/>
-      <c r="H90" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="I90" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="J90" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="K90" s="44" t="s">
+      <c r="D90" s="46"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="47"/>
+      <c r="H90" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="I90" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="J90" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="K90" s="42" t="s">
         <v>0</v>
       </c>
     </row>
@@ -6316,30 +6337,30 @@
     </row>
     <row r="95" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C95" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D95" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E95" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E95" s="9" t="s">
+      <c r="F95" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="F95" s="9" t="s">
+      <c r="G95" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="G95" s="9" t="s">
-        <v>47</v>
-      </c>
       <c r="H95" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I95" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I95" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="J95" s="41">
+      <c r="J95" s="39">
         <v>101</v>
       </c>
-      <c r="K95" s="41">
+      <c r="K95" s="39">
         <v>100</v>
       </c>
     </row>
@@ -6360,51 +6381,51 @@
       <c r="C97" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D97" s="33"/>
-      <c r="E97" s="31"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="31"/>
-      <c r="H97" s="31"/>
-      <c r="I97" s="31"/>
-      <c r="J97" s="31"/>
-      <c r="K97" s="32"/>
-      <c r="L97" s="30" t="s">
+      <c r="D97" s="31"/>
+      <c r="E97" s="29"/>
+      <c r="F97" s="29"/>
+      <c r="G97" s="29"/>
+      <c r="H97" s="29"/>
+      <c r="I97" s="29"/>
+      <c r="J97" s="29"/>
+      <c r="K97" s="30"/>
+      <c r="L97" s="28" t="s">
         <v>22</v>
       </c>
       <c r="M97" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="98" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C98" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="D98" s="45" t="s">
+      <c r="D98" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="E98" s="31"/>
-      <c r="F98" s="31"/>
-      <c r="G98" s="31"/>
-      <c r="H98" s="31"/>
-      <c r="I98" s="31"/>
-      <c r="J98" s="31"/>
-      <c r="K98" s="32"/>
+      <c r="E98" s="29"/>
+      <c r="F98" s="29"/>
+      <c r="G98" s="29"/>
+      <c r="H98" s="29"/>
+      <c r="I98" s="29"/>
+      <c r="J98" s="29"/>
+      <c r="K98" s="30"/>
       <c r="M98" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="99" spans="3:13" x14ac:dyDescent="0.2">
       <c r="C99" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D99" s="42"/>
-      <c r="E99" s="43"/>
-      <c r="F99" s="43"/>
-      <c r="G99" s="43"/>
-      <c r="H99" s="43"/>
-      <c r="I99" s="43"/>
-      <c r="J99" s="43"/>
-      <c r="K99" s="44"/>
+      <c r="D99" s="40"/>
+      <c r="E99" s="41"/>
+      <c r="F99" s="41"/>
+      <c r="G99" s="41"/>
+      <c r="H99" s="41"/>
+      <c r="I99" s="41"/>
+      <c r="J99" s="41"/>
+      <c r="K99" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>